<commit_message>
Factura pdf y modificaciones de alquileres
</commit_message>
<xml_diff>
--- a/Alquileres.xlsx
+++ b/Alquileres.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -29,10 +29,7 @@
     <t>Ubicación entrega</t>
   </si>
   <si>
-    <t>Fecha entrega temprano</t>
-  </si>
-  <si>
-    <t>Fecha entrega Tarde</t>
+    <t>Fecha entrega</t>
   </si>
   <si>
     <t>Usuario cliente</t>
@@ -53,6 +50,9 @@
     <t>Reserva</t>
   </si>
   <si>
+    <t>Precio</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -71,40 +71,97 @@
     <t>16/11/23</t>
   </si>
   <si>
-    <t>17/11/23</t>
+    <t>Tita</t>
+  </si>
+  <si>
+    <t>Emp</t>
+  </si>
+  <si>
+    <t>Loc</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>SUV</t>
+  </si>
+  <si>
+    <t>Elegir</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Gen</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Ruedas</t>
+  </si>
+  <si>
+    <t>Mo</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>05/12/2023</t>
+  </si>
+  <si>
+    <t>06/12/2023</t>
   </si>
   <si>
     <t>Juan</t>
   </si>
   <si>
-    <t>Emp</t>
-  </si>
-  <si>
-    <t>Loc</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>SUV</t>
-  </si>
-  <si>
-    <t>Elegir</t>
-  </si>
-  <si>
-    <t>Gen</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Ruedas</t>
-  </si>
-  <si>
-    <t>Sí</t>
+    <t>100</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>07/12/2023</t>
+  </si>
+  <si>
+    <t>Cli</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>pequeños</t>
+  </si>
+  <si>
+    <t>10/12/2023</t>
+  </si>
+  <si>
+    <t>ExostosXD</t>
+  </si>
+  <si>
+    <t>12/12/2023</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>12000</t>
   </si>
 </sst>
 </file>
@@ -222,13 +279,13 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
@@ -257,22 +314,22 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
         <v>23</v>
@@ -280,7 +337,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -289,7 +346,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -298,36 +355,36 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L4" t="s">
         <v>22</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -336,19 +393,19 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
         <v>20</v>
@@ -357,39 +414,39 @@
         <v>22</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
         <v>20</v>
@@ -398,48 +455,48 @@
         <v>22</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="L7" t="s">
         <v>22</v>
       </c>
       <c r="M7" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tipos de vehículos agregados
</commit_message>
<xml_diff>
--- a/Alquileres.xlsx
+++ b/Alquileres.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Categoría</t>
+    <t>Categoría Y Tipo</t>
   </si>
   <si>
     <t>Fecha recogida</t>
@@ -56,7 +56,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>Pequeños</t>
+    <t>pequeños Automóvil</t>
   </si>
   <si>
     <t>15/11/23</t>
@@ -89,7 +89,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>SUV</t>
+    <t>SUV Automóvil</t>
   </si>
   <si>
     <t>Elegir</t>
@@ -143,9 +143,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>pequeños</t>
-  </si>
-  <si>
     <t>10/12/2023</t>
   </si>
   <si>
@@ -162,6 +159,21 @@
   </si>
   <si>
     <t>12000</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Urbana Bicicleta</t>
+  </si>
+  <si>
+    <t>15/12/2023</t>
+  </si>
+  <si>
+    <t>16/12/2023</t>
+  </si>
+  <si>
+    <t>3000</t>
   </si>
 </sst>
 </file>
@@ -463,19 +475,19 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
       </c>
       <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
         <v>45</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
       </c>
       <c r="G7" t="s">
         <v>36</v>
@@ -484,19 +496,60 @@
         <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" t="s">
         <v>29</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L7" t="s">
         <v>22</v>
       </c>
       <c r="M7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
         <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
App Clientes y correcciones en clases
</commit_message>
<xml_diff>
--- a/Alquileres.xlsx
+++ b/Alquileres.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
   <si>
     <t>Id</t>
   </si>
@@ -80,30 +80,30 @@
     <t>Loc</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>SUV Automóvil</t>
+  </si>
+  <si>
+    <t>Elegir</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Gen</t>
+  </si>
+  <si>
     <t>Sí</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>SUV Automóvil</t>
-  </si>
-  <si>
-    <t>Elegir</t>
-  </si>
-  <si>
-    <t>Martha</t>
-  </si>
-  <si>
-    <t>Gen</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -131,6 +131,9 @@
     <t>5</t>
   </si>
   <si>
+    <t>Naked Moto</t>
+  </si>
+  <si>
     <t>07/12/2023</t>
   </si>
   <si>
@@ -155,9 +158,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>12000</t>
   </si>
   <si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t>3000</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>UTV ATV</t>
+  </si>
+  <si>
+    <t>13/12/2023</t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
 </sst>
 </file>
@@ -382,7 +394,7 @@
         <v>21</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
         <v>23</v>
@@ -423,7 +435,7 @@
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="M5" t="s">
         <v>37</v>
@@ -434,7 +446,7 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -446,13 +458,13 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
@@ -467,45 +479,45 @@
         <v>22</v>
       </c>
       <c r="M6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
         <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
         <v>29</v>
-      </c>
-      <c r="K7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" t="s">
-        <v>22</v>
       </c>
       <c r="M7" t="s">
         <v>48</v>
@@ -537,19 +549,60 @@
         <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="L8" t="s">
         <v>29</v>
       </c>
       <c r="M8" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>